<commit_message>
new work on ground truth
</commit_message>
<xml_diff>
--- a/ground_truth/Règles d'annotation.xlsx
+++ b/ground_truth/Règles d'annotation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Règles d'annotation" sheetId="1" r:id="rId1"/>
+    <sheet name="Cas particuliers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
   <si>
     <t>#</t>
   </si>
@@ -452,6 +453,131 @@
     <t>Si le nom latin d'un ingrédient hors poisson est présent dans la liste des ingrédients, on le conserve.
 Ex : 
 semoule de blé dur blanche biologique (Triticum durum ) &lt;== On conserve Triticum durum</t>
+  </si>
+  <si>
+    <t>Description du cas</t>
+  </si>
+  <si>
+    <t>Fiche technique dont le contenu est en plusieurs langues "mixées"</t>
+  </si>
+  <si>
+    <t>166d4cf3-22f6-4421-85d0-44b1665de41a</t>
+  </si>
+  <si>
+    <t>Fiche technique non renseignée (i.e. avec le format, mais vierge)</t>
+  </si>
+  <si>
+    <t>Fiche technique avec plusieurs composants</t>
+  </si>
+  <si>
+    <t>08e5283e-c269-4b8c-876b-529a5e7fb952</t>
+  </si>
+  <si>
+    <t>Page blanche</t>
+  </si>
+  <si>
+    <t>Fiche technique sans information de composition</t>
+  </si>
+  <si>
+    <t>Fiche technique ne mentionnant les ingrédients que sous forme de tableau</t>
+  </si>
+  <si>
+    <t>Tableau excel pour plusieurs composants</t>
+  </si>
+  <si>
+    <t>Fiche technique en langue étrangère uniquement</t>
+  </si>
+  <si>
+    <t>Fiche technique dont le contenu est en plusieurs langues "séparées"</t>
+  </si>
+  <si>
+    <t>Fiche technique avec des allégations autres que des ingrédients dans le bloc d'ingrédients</t>
+  </si>
+  <si>
+    <t>Fiche technique format image</t>
+  </si>
+  <si>
+    <t>uid exemples</t>
+  </si>
+  <si>
+    <t>4cb8fa90-d588-4901-bfff-124612f2a59f
+8f9f7f4e-da12-4cc2-9d02-b9eb06d659f4</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>Si la liste d'ingrédient mentionne une interprétation de la liste (un synonyme plus parlant), on ne reprend pas cette mention.
+Ex : 
+devient :
+100% tourteau de cacao maigre
+Peut contenir des traces d'arachide et de lait</t>
+  </si>
+  <si>
+    <t>013b</t>
+  </si>
+  <si>
+    <t>S'il existe plusieurs manières différentes de présenter le produit, chacune avec sa liste d'ingrédients, on conserve les 2 de la même manière que lorsqu'il y a plusieurs composants.
+Ex: 
+Vinaigre de vin rouge au jus d’échalote 7% d’acidité
+Vinaigre de vin rouge (sulfites), jus d’échalote (0.5%), arôme*, conservateur: sulfite acide de sodium
+Vinaigre de vin rouge aromatisé à l’échalote 7% d’acidité
+Vinaigre de vin rouge (sulfites), arômes échalote (1%), conservateur: sulfite acide de sodium</t>
+  </si>
+  <si>
+    <t>Fiche technique avec variantes</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>Si une liste d'ingrédient possède une variante en fonction du conditionnement, on conserve les informations relatives à ces précisions.
+Ex : 
+Eau de source*/Eau**; jus de fruits à base de concentrés 12.4% (orange 11.4%, ananas 1%); sucre; acidifiants: acide citrique, acide malique; extraits d’orange; arômes; antioxydant: acide ascorbique; stabilisant: gomme arabique.
+*PET
+**CAN &lt;== On conserve les 2 dernières lignes qui définissent pour quel type de conditionnement la variante s'applique.</t>
+  </si>
+  <si>
+    <t>Fiche technique avec tableau des ingrédients et liste d'ingrédient tel qu'étiqueté</t>
+  </si>
+  <si>
+    <t>0481d91b-9653-42e7-b525-9dc9b87b06f2</t>
+  </si>
+  <si>
+    <t>034c</t>
+  </si>
+  <si>
+    <t>Si une mention précise une condition pour la présence d'additif, on conserve cette mention.
+Ex : 
+INGRÉDIENTS : Segments de pamplemousse, eau, sucre, acidifiant : acide citrique*, agent de fermeté : chlorure de calcium*.
+* En fonction des origines, des additifs peuvent être ajoutés. &lt;== On garde cette mention</t>
+  </si>
+  <si>
+    <t>48bbc56d-563d-4e76-a07d-600d812605f3</t>
+  </si>
+  <si>
+    <t>003b</t>
+  </si>
+  <si>
+    <t>8b87be4b-f966-424a-bbba-76c77fd48464
+aeda7bf1-4d4d-44bb-8518-2e91fc6fd76c</t>
+  </si>
+  <si>
+    <t>b70ed045-57ec-497d-bf18-af14fbbbe955
+(voir les produits VIVIEN PAILLE)
+298053ff-a315-4099-9d2f-eca842508bb3</t>
+  </si>
+  <si>
+    <t>6905af9d-7100-4a96-8a37-007e2a1dfd9f
+6669df16-77f8-4488-bbc2-9c3fe36284f8</t>
+  </si>
+  <si>
+    <t>31411cc4-0629-4493-abab-f6d354811bd8</t>
+  </si>
+  <si>
+    <t>6631c81b-bc5a-4a22-b805-59aaa03cff26
+3eac86f3-abe6-4da3-b292-32133b463538
+e9cecd88-f4f3-4c6c-b518-c715bc2b60e6</t>
   </si>
 </sst>
 </file>
@@ -495,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -505,6 +631,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,13 +664,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>383474</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>482437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>5343896</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1341355</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -567,13 +702,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>61851</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1781300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>6671375</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>2238443</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -605,13 +740,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>284512</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>259773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>8303560</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1678821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -643,13 +778,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>333993</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>210292</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7819707</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>1267435</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -681,13 +816,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>284513</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>272143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>8932132</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>719762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -719,13 +854,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>408214</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>247403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7189166</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>923593</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -745,6 +880,44 @@
         <a:xfrm>
           <a:off x="804058" y="37518604"/>
           <a:ext cx="6780952" cy="676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>395844</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>222662</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4304805</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>706245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="791688" y="42070811"/>
+          <a:ext cx="3908961" cy="483583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1019,11 +1192,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,252 +1326,284 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="43" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1406,4 +1611,170 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finalized work on ground truth
</commit_message>
<xml_diff>
--- a/ground_truth/Règles d'annotation.xlsx
+++ b/ground_truth/Règles d'annotation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Règles d'annotation" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="154">
   <si>
     <t>#</t>
-  </si>
-  <si>
-    <t>Règle</t>
   </si>
   <si>
     <t>001</t>
@@ -92,9 +89,6 @@
     <t>008</t>
   </si>
   <si>
-    <t>On garde les fautes d'orthographe…</t>
-  </si>
-  <si>
     <t>009</t>
   </si>
   <si>
@@ -220,20 +214,6 @@
     <t>022</t>
   </si>
   <si>
-    <t>023</t>
-  </si>
-  <si>
-    <t>De manière générale, on ne retire rien qui est "au milieu" de la liste d'ingrédients.</t>
-  </si>
-  <si>
-    <t>On NE mentionne PAS les réserves relatives au traitement physique.
-Ex : On NE garde PAS ceci
-Malgré tous les soins apportés à nos produits, leur caractère
-naturel n’exclut pas la présence éventuelle de noyaux, de
-pépins, de restes de peaux ou de parties fibreuses.
-Exception : lorsque le cette précision est présent "au milieu" de la liste d'ingrédients.</t>
-  </si>
-  <si>
     <t>024</t>
   </si>
   <si>
@@ -258,18 +238,10 @@
 8e8bbc12-7e4b-4fff-a111-f7c84e35129a</t>
   </si>
   <si>
-    <t>On ne garde pas les préfixes du type "Ingrédients : " ou "Composition :"
-Une exception : lorsque plusieurs composants font l'objet d'une liste d'ingrédients chacun (cf.RG013), on ne retire pas la mention 'Ingrédients :' au milieu du texte.</t>
-  </si>
-  <si>
     <t>027</t>
   </si>
   <si>
     <t>009b</t>
-  </si>
-  <si>
-    <t>Y compris lorsqu'accompagnée de mise en garde particulière : 
-TENEUR ÉLEVÉE EN CAFÉINE, DÉCONSEILLÉ AUX ENFANTS ET AUX FEMMES ENCEINTES OU ALLAITANTES OU AUX PERSONNES SENSIBLES À LA CAFÉINE (21mg/100ml). CONSOMMER AVEC MODÉRATION.</t>
   </si>
   <si>
     <t>En règle générale, on ne récupère que ce qui est mentionné dans le bloc 'Ingrédients' ou 'Composition' de la fiche technique.
@@ -401,14 +373,6 @@
 On ne garde que : ananas, jus d'ananas, antioxydant : acide ascorbique, acidifiant : acide citrique</t>
   </si>
   <si>
-    <t>On garde les précisions relatives au détail de la composition (en particulier le taux de cacao)
-Ex : 
-Taux de coumarine compris entre 1 et 3,5 % ==&gt; on garde
--------------------------------------------------------------------------------------
-sucre, pâte de cacao, beurre de cacao, émulsifiant : lécithine de tournesol (E322), arôme vanille
-cacao : 40%minimum ==&gt; on garde</t>
-  </si>
-  <si>
     <t>037</t>
   </si>
   <si>
@@ -553,38 +517,187 @@
 * En fonction des origines, des additifs peuvent être ajoutés. &lt;== On garde cette mention</t>
   </si>
   <si>
-    <t>48bbc56d-563d-4e76-a07d-600d812605f3</t>
-  </si>
-  <si>
     <t>003b</t>
   </si>
   <si>
-    <t>8b87be4b-f966-424a-bbba-76c77fd48464
-aeda7bf1-4d4d-44bb-8518-2e91fc6fd76c</t>
+    <t>6905af9d-7100-4a96-8a37-007e2a1dfd9f
+6669df16-77f8-4488-bbc2-9c3fe36284f8</t>
+  </si>
+  <si>
+    <t>017b</t>
+  </si>
+  <si>
+    <t>Si une note de bas de page précise la présence d'un composant dans un ingrédient, on le mentionne.
+Ex : 
+Eau, huile de colza, vinaigre d'alcool, MOUTARDE de Dijon (eau, graines de MOUTARDE, vinaigre d'alcool, sel,
+correcteur d'acidité : E330, conservateur : E224*), sel, sucre*, acidifiant : E330, épice, stabilisants : E412 et E415.
+*Contient : SULFITES. &lt;== On garde cette ligne</t>
+  </si>
+  <si>
+    <t>48bbc56d-563d-4e76-a07d-600d812605f3
+f1982954-f091-4aa1-addb-6659062e0f66</t>
+  </si>
+  <si>
+    <t>On garde les précisions relatives au détail de la composition (en particulier le taux de cacao)
+Ex : 
+Taux de coumarine compris entre 1 et 3,5 % ==&gt; on garde
+-------------------------------------------------------------------------------------
+sucre, pâte de cacao, beurre de cacao, émulsifiant : lécithine de tournesol (E322), arôme vanille
+cacao : 40%minimum ==&gt; on garde
+-------------------------------------------------------------------------------------
+chocolat supérieur au lait 39% (sucre, lait en poudre, beurre de cacao, pâte de cacao, émulsifiants : lécithines [soja], vanilline), sucre, lait écrémé en poudre, huile de palme, beurre concentré, émulsifiants : lécithines [soja], vanilline.
+Sur le total : produits laitiers 33 % (lait écrémé en poudre, lait en poudre : 27,4 %, beurre concentré 5,6 %) - cacao 12,5 %. Le chocolat utilisé est un chocolat pur beurre de cacao.  &lt;== On garde cette seconde partie
+-------------------------------------------------------------------------------------
+eau, sirop de glucose-fructose, sucre, épaississant : amidon modifié, graisse végétale non hydrogénée de noix de
+coco, jus concentré de citron 2%, gélifiant : pectines de fruits, arôme naturel de citron, émulsifiants E472C et
+E473, arôme, conservateur : sorbate de potassium, sel, colorant : E161b.
+Teneur en Luteïne : moins de 5 mg/kg &lt;== On garde cette partie</t>
+  </si>
+  <si>
+    <t>Si une note de bas de page précise la variabilité du taux dans la liste d'ingrédients, on conserve cette note.
+Ex : 
+pulpe de pommes (50%)*, sucre, sirop de glucose, gélifiant : pectines, acidifiant : acide citrique, arômes, colorants : E100 - E163 - E160c - E141.
+* Pourcentage à la mise en oeuvre pour chaque parfum. &lt;== On conserve cette ligne.</t>
+  </si>
+  <si>
+    <t>009c</t>
+  </si>
+  <si>
+    <t>035b</t>
+  </si>
+  <si>
+    <t>On conserve les mentions précisant la présence d'un allergène si jamais la liste d'ingrédients ne permet pas de le déduire (sulfites uniquement ?)
+Ex : 
+Huile de colza, « Aceto Balsamico di Modena IGP » (25%) (vinaigre de vin, moût de raisin cuit, colorant E-150d), huile d’olive vierge extra.
+Contient sulfites. &lt;== on garde cette ligne.</t>
+  </si>
+  <si>
+    <t>Etiquette à la place de la fiche technique</t>
+  </si>
+  <si>
+    <t>8dec0469-c9f5-4139-be25-efa258959444</t>
+  </si>
+  <si>
+    <t>7f756c6d-660d-48aa-ad8d-39c03b512ee6</t>
+  </si>
+  <si>
+    <t>Fiche logistique</t>
+  </si>
+  <si>
+    <t>31411cc4-0629-4493-abab-f6d354811bd8
+b29b153c-7244-4bdd-8d36-b5292dcd474b</t>
+  </si>
+  <si>
+    <t>6631c81b-bc5a-4a22-b805-59aaa03cff26
+3eac86f3-abe6-4da3-b292-32133b463538
+e9cecd88-f4f3-4c6c-b518-c715bc2b60e6
+1bc17f58-1530-46e6-aee2-9d302a277420
+8266604c-1ea2-47ca-a4fa-649b4147e733
+8dec0469-c9f5-4139-be25-efa258959444
+a552d585-cb45-43bc-8fb9-1d208485d16c</t>
   </si>
   <si>
     <t>b70ed045-57ec-497d-bf18-af14fbbbe955
 (voir les produits VIVIEN PAILLE)
-298053ff-a315-4099-9d2f-eca842508bb3</t>
-  </si>
-  <si>
-    <t>6905af9d-7100-4a96-8a37-007e2a1dfd9f
-6669df16-77f8-4488-bbc2-9c3fe36284f8</t>
-  </si>
-  <si>
-    <t>31411cc4-0629-4493-abab-f6d354811bd8</t>
-  </si>
-  <si>
-    <t>6631c81b-bc5a-4a22-b805-59aaa03cff26
-3eac86f3-abe6-4da3-b292-32133b463538
-e9cecd88-f4f3-4c6c-b518-c715bc2b60e6</t>
+298053ff-a315-4099-9d2f-eca842508bb3
+64836dd3-5b4f-42ff-862a-31ee19cefda4
+8266604c-1ea2-47ca-a4fa-649b4147e733
+e6fd50ef-8abd-413e-879c-d64b28cbd80a
+93e5d2af-10c5-4853-a437-b013673310cb
+a43ce1f2-76bd-4000-93c6-5b75c5a02d71</t>
+  </si>
+  <si>
+    <t>9fb44f0a-bac3-49e6-a7dc-32257045bad5
+a552d585-cb45-43bc-8fb9-1d208485d16c
+44dca74d-633e-4989-b1b9-2536c832829e</t>
+  </si>
+  <si>
+    <t>addad407-0677-403f-bdf4-a9d3e79bddce
+8b87be4b-f966-424a-bbba-76c77fd48464</t>
+  </si>
+  <si>
+    <t>aeda7bf1-4d4d-44bb-8518-2e91fc6fd76c</t>
+  </si>
+  <si>
+    <t>003c</t>
+  </si>
+  <si>
+    <t>Fiche technique relative à plusieurs produits</t>
+  </si>
+  <si>
+    <t>70500268-802d-4211-93ba-9edbf6e0e7a3</t>
+  </si>
+  <si>
+    <t>MISE EN PAGE ET FORMAT</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>PREFIXES A LA LISTE</t>
+  </si>
+  <si>
+    <t>MENTION DES ALLERGENES</t>
+  </si>
+  <si>
+    <t>On garde les fautes d'orthographe</t>
+  </si>
+  <si>
+    <t>MENTIONS CONDITIONNELLES</t>
+  </si>
+  <si>
+    <t>LISTES D'INGREDIENTS MULTIPLES POUR UNE MEME FICHE TECHNIQUE</t>
+  </si>
+  <si>
+    <t>ORIGINES</t>
+  </si>
+  <si>
+    <t>PRECISIONS SUR LA COMPOSITION - PROPORTIONS</t>
+  </si>
+  <si>
+    <t>PRECISIONS SUR LA COMPOSITION - PRESENCE DE COMPOSANTS SPECIFIQUES HORS ALLERGENES</t>
+  </si>
+  <si>
+    <t>REGLES GENERALES SUR L'INTERPRETATION DU DOCUMENT</t>
+  </si>
+  <si>
+    <t>DETAIL PAR PHASE</t>
+  </si>
+  <si>
+    <t>PRECISION SUR L'IDENTIFICATION D'UN COMPOSANT</t>
+  </si>
+  <si>
+    <t>LABELS DES INGREDIENTS</t>
+  </si>
+  <si>
+    <t>ALLEGATIONS ET RESERVES</t>
+  </si>
+  <si>
+    <t>On NE mentionne PAS les réserves relatives au traitement physique.
+Ex : On NE garde PAS ceci
+Malgré tous les soins apportés à nos produits, leur caractère
+naturel n’exclut pas la présence éventuelle de noyaux, de
+pépins, de restes de peaux ou de parties fibreuses.</t>
+  </si>
+  <si>
+    <t>On ne garde pas les préfixes du type "Ingrédients : " ou "Composition :"</t>
+  </si>
+  <si>
+    <t>LANGUES</t>
+  </si>
+  <si>
+    <t>REGLES DE GESTION</t>
+  </si>
+  <si>
+    <t>Y compris lorsqu'accompagnée de mise en garde particulière : 
+TENEUR ÉLEVÉE EN CAFÉINE, DÉCONSEILLÉ AUX ENFANTS ET AUX FEMMES ENCEINTES OU ALLAITANTES OU AUX PERSONNES SENSIBLES À LA CAFÉINE (21mg/100ml). CONSOMMER AVEC MODÉRATION. &lt;== On garde cette ligne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,13 +713,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -621,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -640,6 +775,15 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,15 +807,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>383474</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>482437</xdr:rowOff>
+      <xdr:colOff>309254</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>482435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5343896</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1341355</xdr:rowOff>
+      <xdr:colOff>5269676</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1341353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -688,7 +832,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="779318" y="23095034"/>
+          <a:off x="705098" y="1991591"/>
           <a:ext cx="4960422" cy="858918"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -701,15 +845,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>61851</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1781300</xdr:rowOff>
+      <xdr:colOff>222664</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1595746</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6671375</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>2238443</xdr:rowOff>
+      <xdr:colOff>6832188</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2052889</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -726,7 +870,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="457695" y="24393897"/>
+          <a:off x="618508" y="3104902"/>
           <a:ext cx="6609524" cy="457143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -739,15 +883,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>284512</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>259773</xdr:rowOff>
+      <xdr:colOff>259771</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>247404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>8303560</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>1678821</xdr:rowOff>
+      <xdr:colOff>8278819</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1666452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -764,7 +908,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="680356" y="29725422"/>
+          <a:off x="655615" y="5566560"/>
           <a:ext cx="8019048" cy="1419048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -777,15 +921,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333993</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>210292</xdr:rowOff>
+      <xdr:colOff>259772</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>235032</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7819707</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>1267435</xdr:rowOff>
+      <xdr:colOff>7745486</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>1292175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -802,7 +946,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="729837" y="31964415"/>
+          <a:off x="655616" y="41266753"/>
           <a:ext cx="7485714" cy="1057143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -815,19 +959,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>284513</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>272143</xdr:rowOff>
+      <xdr:colOff>383474</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>222663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>8932132</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>719762</xdr:rowOff>
+      <xdr:colOff>9031093</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>670282</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6"/>
+        <xdr:cNvPr id="9" name="Image 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -840,7 +984,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="680357" y="36590844"/>
+          <a:off x="779318" y="16353312"/>
           <a:ext cx="8647619" cy="447619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -853,19 +997,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>408214</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>309254</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>247403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7189166</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>7090206</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>923593</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7"/>
+        <xdr:cNvPr id="10" name="Image 9"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -878,7 +1022,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="804058" y="37518604"/>
+          <a:off x="705098" y="8040585"/>
           <a:ext cx="6780952" cy="676190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -891,19 +1035,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>395844</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>222662</xdr:rowOff>
+      <xdr:colOff>321624</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>210292</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4304805</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>706245</xdr:rowOff>
+      <xdr:colOff>4230585</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>693875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 5"/>
+        <xdr:cNvPr id="11" name="Image 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -916,7 +1060,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="791688" y="42070811"/>
+          <a:off x="717468" y="7248896"/>
           <a:ext cx="3908961" cy="483583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1192,11 +1336,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,404 +1352,532 @@
     <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1615,10 +1889,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,152 +1903,194 @@
     <col min="1" max="1" width="5.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="82.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="4"/>
+    <col min="4" max="5" width="11.42578125" style="4"/>
+    <col min="6" max="6" width="40.5703125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C9" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C11" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C16" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>